<commit_message>
added user as trip_mate pledges
</commit_message>
<xml_diff>
--- a/project-details/crowdfunding_project_traveld.xlsx
+++ b/project-details/crowdfunding_project_traveld.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gianr9\Desktop\SheCodes\project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gianr9\Desktop\SheCodes\traveld\project-details\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="132">
   <si>
     <t>Trip</t>
   </si>
@@ -95,9 +95,6 @@
     <t>/pledges/1</t>
   </si>
   <si>
-    <t>Return all trips</t>
-  </si>
-  <si>
     <t>Create a new trip</t>
   </si>
   <si>
@@ -117,9 +114,6 @@
   </si>
   <si>
     <t>/trips/1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Return trips with ID of “1”. </t>
   </si>
   <si>
     <t xml:space="preserve">Return pledge with ID of “1”. </t>
@@ -403,16 +397,34 @@
     <t>URL not found</t>
   </si>
   <si>
-    <t>Created a new trip with missing field</t>
-  </si>
-  <si>
     <t>400 Bad Request</t>
   </si>
   <si>
-    <t>Created a new pledge with missing field</t>
-  </si>
-  <si>
-    <t>pledge object</t>
+    <t xml:space="preserve">Get Trip details with ID of “1”. </t>
+  </si>
+  <si>
+    <t>Return all trips - Get list of trips</t>
+  </si>
+  <si>
+    <t>/api-token-auth/</t>
+  </si>
+  <si>
+    <t>Create User Token</t>
+  </si>
+  <si>
+    <t>Failure Response Code</t>
+  </si>
+  <si>
+    <t>/trips/10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Delets trip with ID of “10”.  </t>
+  </si>
+  <si>
+    <t>/pledges</t>
+  </si>
+  <si>
+    <t>Return all pledges - Get list of pledges</t>
   </si>
 </sst>
 </file>
@@ -465,7 +477,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -511,6 +523,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -701,7 +719,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
@@ -800,9 +818,6 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -814,6 +829,31 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1381,7 +1421,7 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="50" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B1" s="42"/>
       <c r="C1" s="42"/>
@@ -1413,7 +1453,7 @@
       <c r="E3" s="42"/>
       <c r="F3" s="42"/>
       <c r="G3" s="10" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="H3" s="11"/>
       <c r="I3" s="29"/>
@@ -1450,17 +1490,17 @@
       <c r="D5" s="42"/>
       <c r="E5" s="42"/>
       <c r="F5" s="42"/>
-      <c r="G5" s="53" t="s">
-        <v>94</v>
-      </c>
-      <c r="H5" s="54" t="s">
+      <c r="G5" s="52" t="s">
+        <v>92</v>
+      </c>
+      <c r="H5" s="53" t="s">
         <v>7</v>
       </c>
       <c r="I5" s="29"/>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>10</v>
@@ -1470,7 +1510,7 @@
       <c r="E6" s="42"/>
       <c r="F6" s="42"/>
       <c r="G6" s="26" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="H6" s="2" t="s">
         <v>7</v>
@@ -1479,7 +1519,7 @@
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>7</v>
@@ -1489,7 +1529,7 @@
       <c r="E7" s="42"/>
       <c r="F7" s="42"/>
       <c r="G7" s="16" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="H7" s="17" t="s">
         <v>7</v>
@@ -1498,7 +1538,7 @@
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>8</v>
@@ -1508,7 +1548,7 @@
       <c r="E8" s="42"/>
       <c r="F8" s="42"/>
       <c r="G8" s="27" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H8" s="19" t="s">
         <v>9</v>
@@ -1527,7 +1567,7 @@
       <c r="E9" s="42"/>
       <c r="F9" s="42"/>
       <c r="G9" s="46" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="H9" s="47" t="s">
         <v>7</v>
@@ -1546,7 +1586,7 @@
       <c r="E10" s="42"/>
       <c r="F10" s="42"/>
       <c r="G10" s="48" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="H10" s="49" t="s">
         <v>7</v>
@@ -1602,7 +1642,7 @@
     </row>
     <row r="14" spans="1:9" ht="15" thickBot="1">
       <c r="A14" s="8" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B14" s="9" t="s">
         <v>7</v>
@@ -1620,7 +1660,7 @@
       <c r="B15" s="42"/>
       <c r="C15" s="42"/>
       <c r="D15" s="10" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E15" s="11"/>
       <c r="G15" s="42"/>
@@ -1649,7 +1689,7 @@
       <c r="B17" s="42"/>
       <c r="C17" s="42"/>
       <c r="D17" s="14" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E17" s="15" t="s">
         <v>8</v>
@@ -1664,7 +1704,7 @@
       <c r="B18" s="42"/>
       <c r="C18" s="42"/>
       <c r="D18" s="16" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E18" s="17" t="s">
         <v>8</v>
@@ -1679,7 +1719,7 @@
       <c r="B19" s="42"/>
       <c r="C19" s="42"/>
       <c r="D19" s="16" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E19" s="17" t="s">
         <v>8</v>
@@ -1709,7 +1749,7 @@
       <c r="B21" s="42"/>
       <c r="C21" s="42"/>
       <c r="D21" s="18" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E21" s="19" t="s">
         <v>8</v>
@@ -1770,41 +1810,43 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col min="1" max="1" width="13.3984375" customWidth="1"/>
-    <col min="2" max="2" width="12.8984375" customWidth="1"/>
+    <col min="2" max="2" width="14.59765625" customWidth="1"/>
     <col min="3" max="3" width="33.3984375" customWidth="1"/>
     <col min="4" max="4" width="17.296875" customWidth="1"/>
-    <col min="5" max="5" width="23.796875" customWidth="1"/>
-    <col min="6" max="6" width="30.09765625" customWidth="1"/>
+    <col min="5" max="6" width="23.796875" customWidth="1"/>
+    <col min="7" max="7" width="30.09765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7">
       <c r="A1" s="28" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B1" s="29"/>
       <c r="C1" s="29"/>
       <c r="D1" s="29"/>
       <c r="E1" s="29"/>
       <c r="F1" s="29"/>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="G1" s="29"/>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2" s="29"/>
       <c r="B2" s="29"/>
       <c r="C2" s="29"/>
       <c r="D2" s="29"/>
       <c r="E2" s="29"/>
       <c r="F2" s="29"/>
-    </row>
-    <row r="3" spans="1:6" ht="29.4" customHeight="1">
+      <c r="G2" s="29"/>
+    </row>
+    <row r="3" spans="1:7" ht="29.4" customHeight="1">
       <c r="A3" s="20" t="s">
         <v>12</v>
       </c>
@@ -1815,333 +1857,391 @@
         <v>18</v>
       </c>
       <c r="D3" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3" s="21" t="s">
+        <v>127</v>
+      </c>
+      <c r="G3" s="22" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="29.4" customHeight="1">
+      <c r="A4" s="61" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="61" t="s">
+        <v>125</v>
+      </c>
+      <c r="C4" s="61" t="s">
+        <v>126</v>
+      </c>
+      <c r="D4" s="61" t="s">
+        <v>54</v>
+      </c>
+      <c r="E4" s="62">
+        <v>200</v>
+      </c>
+      <c r="F4" s="62" t="s">
+        <v>122</v>
+      </c>
+      <c r="G4" s="54" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="29.4" customHeight="1">
+      <c r="A5" s="54" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="54" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="54" t="s">
+        <v>124</v>
+      </c>
+      <c r="D5" s="54" t="s">
         <v>25</v>
       </c>
-      <c r="E3" s="21" t="s">
+      <c r="E5" s="55">
+        <v>200</v>
+      </c>
+      <c r="F5" s="55" t="s">
+        <v>122</v>
+      </c>
+      <c r="G5" s="54" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="29.4" customHeight="1">
+      <c r="A6" s="54" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="54" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="54" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="54" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" s="55">
+        <v>201</v>
+      </c>
+      <c r="F6" s="55" t="s">
+        <v>122</v>
+      </c>
+      <c r="G6" s="54" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="29.4" customHeight="1">
+      <c r="A7" s="54" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="54" t="s">
         <v>28</v>
       </c>
-      <c r="F3" s="22" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="29.4" customHeight="1">
-      <c r="A4" s="55" t="s">
+      <c r="C7" s="54" t="s">
+        <v>123</v>
+      </c>
+      <c r="D7" s="54" t="s">
+        <v>25</v>
+      </c>
+      <c r="E7" s="55">
+        <v>200</v>
+      </c>
+      <c r="F7" s="55" t="s">
+        <v>122</v>
+      </c>
+      <c r="G7" s="54" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="29.4" customHeight="1">
+      <c r="A8" s="54" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="54" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" s="54" t="s">
+        <v>59</v>
+      </c>
+      <c r="D8" s="54" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8" s="55">
+        <v>201</v>
+      </c>
+      <c r="F8" s="55" t="s">
+        <v>122</v>
+      </c>
+      <c r="G8" s="56" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="29.4" customHeight="1">
+      <c r="A9" s="54" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="54" t="s">
+        <v>128</v>
+      </c>
+      <c r="C9" s="54" t="s">
+        <v>129</v>
+      </c>
+      <c r="D9" s="54" t="s">
+        <v>26</v>
+      </c>
+      <c r="E9" s="55">
+        <v>200</v>
+      </c>
+      <c r="F9" s="55" t="s">
+        <v>122</v>
+      </c>
+      <c r="G9" s="56" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="29.4" customHeight="1">
+      <c r="A10" s="54" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="55" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" s="55" t="s">
-        <v>22</v>
-      </c>
-      <c r="D4" s="55" t="s">
+      <c r="B10" s="54" t="s">
+        <v>130</v>
+      </c>
+      <c r="C10" s="54" t="s">
+        <v>131</v>
+      </c>
+      <c r="D10" s="54" t="s">
+        <v>25</v>
+      </c>
+      <c r="E10" s="55">
+        <v>200</v>
+      </c>
+      <c r="F10" s="55" t="s">
+        <v>122</v>
+      </c>
+      <c r="G10" s="54" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="29.4" customHeight="1">
+      <c r="A11" s="63" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="63" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="63" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" s="63" t="s">
         <v>26</v>
       </c>
-      <c r="E4" s="56">
+      <c r="E11" s="64">
+        <v>201</v>
+      </c>
+      <c r="F11" s="64" t="s">
+        <v>122</v>
+      </c>
+      <c r="G11" s="65" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="29.4" customHeight="1">
+      <c r="A12" s="63" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="63" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="63" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12" s="63" t="s">
+        <v>25</v>
+      </c>
+      <c r="E12" s="64">
         <v>200</v>
       </c>
-      <c r="F4" s="55" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="29.4" customHeight="1">
-      <c r="A5" s="55" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" s="55" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" s="55" t="s">
-        <v>23</v>
-      </c>
-      <c r="D5" s="55" t="s">
-        <v>27</v>
-      </c>
-      <c r="E5" s="56">
-        <v>201</v>
-      </c>
-      <c r="F5" s="23" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="29.4" customHeight="1">
-      <c r="A6" s="55" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" s="55" t="s">
-        <v>29</v>
-      </c>
-      <c r="C6" s="55" t="s">
-        <v>30</v>
-      </c>
-      <c r="D6" s="55" t="s">
-        <v>26</v>
-      </c>
-      <c r="E6" s="56">
-        <v>200</v>
-      </c>
-      <c r="F6" s="23" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="29.4" customHeight="1">
-      <c r="A7" s="23" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" s="23" t="s">
-        <v>29</v>
-      </c>
-      <c r="C7" s="23" t="s">
-        <v>61</v>
-      </c>
-      <c r="D7" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="E7" s="24">
-        <v>201</v>
-      </c>
-      <c r="F7" s="25" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="29.4" customHeight="1">
-      <c r="A8" s="55" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" s="55" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" s="55" t="s">
-        <v>24</v>
-      </c>
-      <c r="D8" s="55" t="s">
-        <v>27</v>
-      </c>
-      <c r="E8" s="56">
-        <v>201</v>
-      </c>
-      <c r="F8" s="25" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="29.4" customHeight="1">
-      <c r="A9" s="55" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" s="55" t="s">
-        <v>21</v>
-      </c>
-      <c r="C9" s="55" t="s">
+      <c r="F12" s="64" t="s">
+        <v>122</v>
+      </c>
+      <c r="G12" s="63" t="s">
         <v>31</v>
       </c>
-      <c r="D9" s="55" t="s">
-        <v>26</v>
-      </c>
-      <c r="E9" s="56">
-        <v>200</v>
-      </c>
-      <c r="F9" s="23" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="29.4" customHeight="1">
-      <c r="A10" s="23" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10" s="23" t="s">
-        <v>21</v>
-      </c>
-      <c r="C10" s="23" t="s">
-        <v>59</v>
-      </c>
-      <c r="D10" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="E10" s="24">
-        <v>200</v>
-      </c>
-      <c r="F10" s="25" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="29.4" customHeight="1">
-      <c r="A11" s="23" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" s="23" t="s">
-        <v>51</v>
-      </c>
-      <c r="C11" s="23" t="s">
-        <v>55</v>
-      </c>
-      <c r="D11" s="23" t="s">
-        <v>56</v>
-      </c>
-      <c r="E11" s="24">
-        <v>201</v>
-      </c>
-      <c r="F11" s="25" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="29.4" customHeight="1">
-      <c r="A12" s="23" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" s="23" t="s">
-        <v>52</v>
-      </c>
-      <c r="C12" s="23" t="s">
-        <v>53</v>
-      </c>
-      <c r="D12" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="E12" s="24">
-        <v>200</v>
-      </c>
-      <c r="F12" s="23" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="29.4" customHeight="1">
+    </row>
+    <row r="13" spans="1:7" ht="29.4" customHeight="1">
       <c r="A13" s="23" t="s">
         <v>16</v>
       </c>
       <c r="B13" s="23" t="s">
-        <v>52</v>
+        <v>21</v>
       </c>
       <c r="C13" s="23" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="D13" s="23" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E13" s="24">
         <v>200</v>
       </c>
-      <c r="F13" s="25" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="28.2" customHeight="1">
+      <c r="F13" s="24"/>
+      <c r="G13" s="25" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="29.4" customHeight="1">
       <c r="A14" s="23" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B14" s="23" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C14" s="23" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="D14" s="23" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E14" s="24">
         <v>201</v>
       </c>
-      <c r="F14" s="25" t="s">
+      <c r="F14" s="24"/>
+      <c r="G14" s="25" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="29.4" customHeight="1">
+      <c r="A15" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="C15" s="23" t="s">
+        <v>51</v>
+      </c>
+      <c r="D15" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="E15" s="24">
+        <v>200</v>
+      </c>
+      <c r="F15" s="24"/>
+      <c r="G15" s="23" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="28.2" customHeight="1">
+      <c r="A16" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="C16" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="D16" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="E16" s="24">
+        <v>200</v>
+      </c>
+      <c r="F16" s="24"/>
+      <c r="G16" s="25" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="28.2" customHeight="1">
+      <c r="A17" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="C17" s="23" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" ht="28.2" customHeight="1">
-      <c r="A15" s="23" t="s">
+      <c r="D17" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="E17" s="24">
+        <v>201</v>
+      </c>
+      <c r="F17" s="24"/>
+      <c r="G17" s="25" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="28.2" customHeight="1">
+      <c r="A18" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="23" t="s">
-        <v>63</v>
-      </c>
-      <c r="C15" s="23" t="s">
-        <v>60</v>
-      </c>
-      <c r="D15" s="23" t="s">
-        <v>56</v>
-      </c>
-      <c r="E15" s="24">
+      <c r="B18" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="C18" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="D18" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="E18" s="24">
         <v>201</v>
       </c>
-      <c r="F15" s="25" t="s">
+      <c r="F18" s="24"/>
+      <c r="G18" s="25" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="28.2" customHeight="1">
+      <c r="A19" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="B19" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="C19" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="D19" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="E19" s="24">
+        <v>201</v>
+      </c>
+      <c r="F19" s="24"/>
+      <c r="G19" s="25" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20" s="58" t="s">
+        <v>13</v>
+      </c>
+      <c r="B20" s="58" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" ht="28.2" customHeight="1">
-      <c r="A16" s="23" t="s">
-        <v>15</v>
-      </c>
-      <c r="B16" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="C16" s="23" t="s">
-        <v>60</v>
-      </c>
-      <c r="D16" s="23" t="s">
-        <v>56</v>
-      </c>
-      <c r="E16" s="24">
-        <v>201</v>
-      </c>
-      <c r="F16" s="25" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="28.2" customHeight="1">
-      <c r="A17" s="55" t="s">
-        <v>13</v>
-      </c>
-      <c r="B17" s="55" t="s">
-        <v>122</v>
-      </c>
-      <c r="C17" s="55" t="s">
-        <v>123</v>
-      </c>
-      <c r="D17" s="55" t="s">
-        <v>26</v>
-      </c>
-      <c r="E17" s="56">
+      <c r="C20" s="58" t="s">
+        <v>121</v>
+      </c>
+      <c r="D20" s="58" t="s">
+        <v>25</v>
+      </c>
+      <c r="E20" s="59">
         <v>404</v>
       </c>
-      <c r="F17" s="57" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="28.2" customHeight="1">
-      <c r="A18" s="55" t="s">
-        <v>14</v>
-      </c>
-      <c r="B18" s="55" t="s">
-        <v>19</v>
-      </c>
-      <c r="C18" s="55" t="s">
-        <v>124</v>
-      </c>
-      <c r="D18" s="55" t="s">
-        <v>27</v>
-      </c>
-      <c r="E18" s="56" t="s">
-        <v>125</v>
-      </c>
-      <c r="F18" s="25" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="28.2" customHeight="1">
-      <c r="A19" s="55" t="s">
-        <v>14</v>
-      </c>
-      <c r="B19" s="55" t="s">
-        <v>20</v>
-      </c>
-      <c r="C19" s="55" t="s">
-        <v>126</v>
-      </c>
-      <c r="D19" s="55" t="s">
-        <v>127</v>
-      </c>
-      <c r="E19" s="56" t="s">
-        <v>125</v>
-      </c>
-      <c r="F19" s="25" t="s">
-        <v>34</v>
+      <c r="F20" s="59"/>
+      <c r="G20" s="60" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -2166,12 +2266,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="52" t="s">
-        <v>66</v>
-      </c>
-      <c r="B1" s="52"/>
+      <c r="A1" s="57" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" s="57"/>
       <c r="C1" s="28" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D1" s="29"/>
     </row>
@@ -2183,21 +2283,21 @@
     </row>
     <row r="3" spans="1:4" ht="21.6" customHeight="1">
       <c r="A3" s="30" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B3" s="30"/>
       <c r="C3" s="31" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D3" s="29"/>
     </row>
     <row r="4" spans="1:4" ht="35.4" customHeight="1">
       <c r="A4" s="30" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B4" s="30"/>
       <c r="C4" s="32" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D4" s="29"/>
     </row>
@@ -2209,11 +2309,11 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="28" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B6" s="28"/>
       <c r="C6" s="28" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D6" s="29"/>
     </row>
@@ -2221,7 +2321,7 @@
       <c r="A7" s="29"/>
       <c r="B7" s="29"/>
       <c r="C7" s="33" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D7" s="29"/>
     </row>
@@ -2229,7 +2329,7 @@
       <c r="A8" s="29"/>
       <c r="B8" s="29"/>
       <c r="C8" s="33" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D8" s="29"/>
     </row>
@@ -2237,7 +2337,7 @@
       <c r="A9" s="29"/>
       <c r="B9" s="29"/>
       <c r="C9" s="33" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D9" s="29"/>
     </row>
@@ -2245,7 +2345,7 @@
       <c r="A10" s="29"/>
       <c r="B10" s="29"/>
       <c r="C10" s="28" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D10" s="29"/>
     </row>
@@ -2253,7 +2353,7 @@
       <c r="A11" s="29"/>
       <c r="B11" s="29"/>
       <c r="C11" s="29" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D11" s="29"/>
     </row>
@@ -2261,7 +2361,7 @@
       <c r="A12" s="29"/>
       <c r="B12" s="29"/>
       <c r="C12" s="33" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D12" s="29"/>
     </row>
@@ -2269,7 +2369,7 @@
       <c r="A13" s="29"/>
       <c r="B13" s="29"/>
       <c r="C13" s="33" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D13" s="29"/>
     </row>
@@ -2277,7 +2377,7 @@
       <c r="A14" s="29"/>
       <c r="B14" s="29"/>
       <c r="C14" s="33" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D14" s="29"/>
     </row>
@@ -2285,7 +2385,7 @@
       <c r="A15" s="29"/>
       <c r="B15" s="29"/>
       <c r="C15" s="33" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D15" s="29"/>
     </row>
@@ -2301,7 +2401,7 @@
       <c r="A17" s="29"/>
       <c r="B17" s="29"/>
       <c r="C17" s="29" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D17" s="29"/>
     </row>
@@ -2309,7 +2409,7 @@
       <c r="A18" s="29"/>
       <c r="B18" s="29"/>
       <c r="C18" s="29" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D18" s="29"/>
     </row>
@@ -2317,7 +2417,7 @@
       <c r="A19" s="29"/>
       <c r="B19" s="29"/>
       <c r="C19" s="34" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D19" s="29"/>
     </row>
@@ -2331,7 +2431,7 @@
       <c r="A21" s="29"/>
       <c r="B21" s="29"/>
       <c r="C21" s="28" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D21" s="29"/>
     </row>
@@ -2339,7 +2439,7 @@
       <c r="A22" s="29"/>
       <c r="B22" s="29"/>
       <c r="C22" s="29" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D22" s="29"/>
     </row>
@@ -2347,7 +2447,7 @@
       <c r="A23" s="29"/>
       <c r="B23" s="29"/>
       <c r="C23" s="35" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D23" s="29"/>
     </row>
@@ -2355,7 +2455,7 @@
       <c r="A24" s="29"/>
       <c r="B24" s="29"/>
       <c r="C24" s="35" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D24" s="29"/>
     </row>
@@ -2363,7 +2463,7 @@
       <c r="A25" s="29"/>
       <c r="B25" s="29"/>
       <c r="C25" s="35" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D25" s="29"/>
     </row>
@@ -2371,7 +2471,7 @@
       <c r="A26" s="29"/>
       <c r="B26" s="29"/>
       <c r="C26" s="35" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D26" s="29"/>
     </row>
@@ -2379,7 +2479,7 @@
       <c r="A27" s="29"/>
       <c r="B27" s="29"/>
       <c r="C27" s="35" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D27" s="29"/>
     </row>
@@ -2387,7 +2487,7 @@
       <c r="A28" s="29"/>
       <c r="B28" s="29"/>
       <c r="C28" s="35" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D28" s="29"/>
     </row>
@@ -2395,7 +2495,7 @@
       <c r="A29" s="29"/>
       <c r="B29" s="29"/>
       <c r="C29" s="35" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D29" s="29"/>
     </row>
@@ -2403,7 +2503,7 @@
       <c r="A30" s="29"/>
       <c r="B30" s="29"/>
       <c r="C30" s="35" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D30" s="29"/>
     </row>
@@ -2411,7 +2511,7 @@
       <c r="A31" s="29"/>
       <c r="B31" s="29"/>
       <c r="C31" s="35" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D31" s="29"/>
     </row>
@@ -2419,7 +2519,7 @@
       <c r="A32" s="29"/>
       <c r="B32" s="29"/>
       <c r="C32" s="35" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D32" s="29"/>
     </row>
@@ -2427,14 +2527,14 @@
       <c r="A33" s="29"/>
       <c r="B33" s="29"/>
       <c r="C33" s="34" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D33" s="29"/>
     </row>
     <row r="34" spans="1:4">
       <c r="B34" s="29"/>
       <c r="C34" s="34" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D34" s="29"/>
     </row>
@@ -2442,7 +2542,7 @@
       <c r="A35" s="29"/>
       <c r="B35" s="29"/>
       <c r="C35" s="34" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D35" s="29"/>
     </row>
@@ -2450,7 +2550,7 @@
       <c r="A36" s="29"/>
       <c r="B36" s="29"/>
       <c r="C36" s="34" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D36" s="29"/>
     </row>
@@ -2458,7 +2558,7 @@
       <c r="A37" s="29"/>
       <c r="B37" s="29"/>
       <c r="C37" s="34" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D37" s="29"/>
     </row>
@@ -2466,7 +2566,7 @@
       <c r="A38" s="29"/>
       <c r="B38" s="29"/>
       <c r="C38" s="34" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D38" s="29"/>
     </row>
@@ -2480,7 +2580,7 @@
       <c r="A40" s="29"/>
       <c r="B40" s="29"/>
       <c r="C40" s="36" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D40" s="29"/>
     </row>
@@ -2488,7 +2588,7 @@
       <c r="A41" s="29"/>
       <c r="B41" s="29"/>
       <c r="C41" s="34" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D41" s="29"/>
     </row>
@@ -2496,7 +2596,7 @@
       <c r="A42" s="29"/>
       <c r="B42" s="29"/>
       <c r="C42" s="33" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D42" s="29"/>
     </row>
@@ -2504,17 +2604,17 @@
       <c r="A43" s="29"/>
       <c r="B43" s="29"/>
       <c r="C43" s="33" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D43" s="29"/>
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="28" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B44" s="28"/>
       <c r="C44" s="33" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D44" s="29"/>
     </row>
@@ -2522,7 +2622,7 @@
       <c r="A45" s="29"/>
       <c r="B45" s="29"/>
       <c r="C45" s="33" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D45" s="29"/>
     </row>
@@ -2530,7 +2630,7 @@
       <c r="A46" s="29"/>
       <c r="B46" s="29"/>
       <c r="C46" s="34" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D46" s="29"/>
     </row>
@@ -2544,7 +2644,7 @@
       <c r="A48" s="29"/>
       <c r="B48" s="29"/>
       <c r="C48" s="37" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D48" s="29"/>
     </row>
@@ -2552,7 +2652,7 @@
       <c r="A49" s="29"/>
       <c r="B49" s="29"/>
       <c r="C49" s="29" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D49" s="29"/>
     </row>
@@ -2560,7 +2660,7 @@
       <c r="A50" s="29"/>
       <c r="B50" s="29"/>
       <c r="C50" s="29" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D50" s="29"/>
     </row>
@@ -2568,7 +2668,7 @@
       <c r="A51" s="29"/>
       <c r="B51" s="29"/>
       <c r="C51" s="29" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D51" s="29"/>
     </row>
@@ -2608,7 +2708,7 @@
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="28" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B2" s="29"/>
       <c r="C2" s="29"/>
@@ -2623,10 +2723,10 @@
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="38" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B3" s="29" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C3" s="29"/>
       <c r="D3" s="29"/>
@@ -2640,10 +2740,10 @@
     </row>
     <row r="4" spans="1:11">
       <c r="A4" s="28" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B4" s="29" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C4" s="29"/>
       <c r="D4" s="29"/>
@@ -2657,7 +2757,7 @@
     </row>
     <row r="5" spans="1:11">
       <c r="A5" s="39" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B5" s="29"/>
       <c r="C5" s="29"/>
@@ -2854,7 +2954,7 @@
     </row>
     <row r="20" spans="1:11">
       <c r="A20" s="28" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B20" s="29"/>
       <c r="C20" s="29"/>

</xml_diff>